<commit_message>
Update Cannot lock C:\Users\rohit.kashyap\git\repository\.git\index. Ensure that no other process has an open file handle on the lock file C:\Users\rohit.kashyap\git\repository\.git\index.lock, then you may delete the lock file and retry. Cannot lock C:\Users\rohit.kashyap\git\repository\.git\index. Ensure that no other process has an open file handle on the lock file C:\Users\rohit.kashyap\git\repository\.git\index.lock, then you may delete the lock file and retry.Cannot lock C:\Users\rohit.kashyap\git\repository\.git\index. Ensure that no other process has an open file handle on the lock file C:\Users\rohit.kashyap\git\repository\.git\index.lock, then you may delete the lock file and retry. Cannot lock C:\Users\rohit.kashyap\git\repository\.git\index. Ensure that no other process has an open file handle on the lock file C:\Users\rohit.kashyap\git\repository\.git\index.lock, then you may delete the lock file and retry.
</commit_message>
<xml_diff>
--- a/expobazaar/Test_data/Test_data.xlsx
+++ b/expobazaar/Test_data/Test_data.xlsx
@@ -3,16 +3,16 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20397"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{867D013A-0E5F-4B4C-9603-7A804982C842}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{1BB116B7-837F-4C19-A69C-586651DB390B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11610" windowHeight="3225" xr2:uid="{861E9007-179A-411A-95A5-EBA08FB71D6E}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11550" windowHeight="2115" activeTab="1" xr2:uid="{861E9007-179A-411A-95A5-EBA08FB71D6E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
+  <oleSize ref="A1:J4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -414,7 +414,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63BEC13E-55F1-43D3-A348-08B0E8B57C94}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
@@ -475,7 +475,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03575717-09D9-4A59-95AF-A7A22721DCF3}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="115" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>

</xml_diff>